<commit_message>
updated power BOM and total cost
</commit_message>
<xml_diff>
--- a/Production/POWER_MODULE_v3.xlsx
+++ b/Production/POWER_MODULE_v3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vuyisa\Documents\kiCAD\sensor\EEE3088_PROJECT\EEE3088_PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vuyisa\MAIN_PROJECT\eee3088f-project\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B07F8F-C194-431F-82F3-462F5900D94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D863EFE5-2FA0-44B5-9CA3-0E8F661E4E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DDA5B56F-5668-4194-88F0-FF7F5B786AA7}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>MCP1700-3302E_TO92</t>
   </si>
   <si>
-    <t>ReferenceValue</t>
-  </si>
-  <si>
     <t>JLCPCB Part</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>C1002</t>
   </si>
   <si>
-    <t>battery holder</t>
-  </si>
-  <si>
     <t>C69335</t>
   </si>
   <si>
@@ -218,6 +212,12 @@
   </si>
   <si>
     <t>C132560</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -328,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B36DB25-DC13-4AC1-B0AF-E4CCD97D0DB9}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowCount="1">
-  <autoFilter ref="A1:F21" xr:uid="{2B36DB25-DC13-4AC1-B0AF-E4CCD97D0DB9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B36DB25-DC13-4AC1-B0AF-E4CCD97D0DB9}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowCount="1">
+  <autoFilter ref="A1:F20" xr:uid="{2B36DB25-DC13-4AC1-B0AF-E4CCD97D0DB9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9E85547D-D76C-4EB6-9A8F-9B51C5E5802F}" name="Column1" totalsRowLabel="TOTAL PRICE($)"/>
     <tableColumn id="2" xr3:uid="{10EC5C1B-A6E2-49A3-9DE6-7A5A47A99113}" name="Column2"/>
@@ -337,7 +337,7 @@
     <tableColumn id="4" xr3:uid="{2E26A0BB-DC22-4372-8075-022268C7730D}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{CAE5847F-DBB0-495B-9596-158D17098424}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{E168FF96-8DD7-4C63-B936-832F64EE2FFB}" name="Column6" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(F2:F21)</totalsRowFormula>
+      <totalsRowFormula>SUM(F2:F20)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -641,52 +641,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ACCC2F-368D-430F-8361-F9CE025C2F6F}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="11" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -709,276 +716,282 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
       </c>
       <c r="D4">
-        <v>4.18</v>
+        <v>2.0299999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F21" si="0">PRODUCT(D4:E4)</f>
-        <v>4.18</v>
+        <f t="shared" ref="F4:F20" si="0">PRODUCT(D4:E4)</f>
+        <v>4.0599999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5">
-        <v>2.0299999999999999E-2</v>
+        <v>42</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>4.0599999999999997E-2</v>
+        <v>1.1599999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="5">
-        <v>5.7999999999999996E-3</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>1.1599999999999999E-2</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.1000000000000001E-3</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>2.0299999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>5.1999999999999998E-3</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D9">
-        <v>2.0299999999999999E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>2.0299999999999999E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10">
-        <v>3.2000000000000002E-3</v>
+      <c r="D10" s="6">
+        <v>0.83299999999999996</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>3.2000000000000002E-3</v>
+        <v>1.6659999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.83299999999999996</v>
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>1.6659999999999999</v>
+        <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="9">
-        <v>5.1999999999999998E-3</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.35149999999999998</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>5.1999999999999998E-3</v>
+        <v>0.35149999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.35149999999999998</v>
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.35149999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.73629999999999995</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.73629999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>22</v>
+      <c r="A15" s="1">
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.73629999999999995</v>
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.95E-2</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.73629999999999995</v>
+        <v>1.95E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="3">
-        <v>1.95E-2</v>
+      <c r="D16" s="7">
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>1.95E-2</v>
+        <v>1.2999999999999999E-3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="7">
@@ -993,96 +1006,75 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="1">
-        <v>4</v>
+      <c r="A18" t="s">
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1.2999999999999999E-3</v>
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>1.3166</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>1.2999999999999999E-3</v>
+        <v>1.3166</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19">
-        <v>1.3166</v>
+        <v>45</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6.6311999999999998</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1.3166</v>
+        <v>6.6311999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="7">
-        <v>6.6311999999999998</v>
+      <c r="D20" s="3">
+        <v>0.96099999999999997</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>6.6311999999999998</v>
+        <v>0.96099999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0.96099999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22">
-        <f>SUM(F2:F21)</f>
-        <v>15.951899999999998</v>
+        <f>SUM(F2:F20)</f>
+        <v>11.7719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>